<commit_message>
Added 1.1.0 version of data
</commit_message>
<xml_diff>
--- a/2021/district_councils.xlsx
+++ b/2021/district_councils.xlsx
@@ -166,12 +166,12 @@
     <t>Thanet District Council</t>
   </si>
   <si>
+    <t>Babergh District Council</t>
+  </si>
+  <si>
     <t>Mid Suffolk District Council</t>
   </si>
   <si>
-    <t>Babergh District Council</t>
-  </si>
-  <si>
     <t>Mid Devon District Council</t>
   </si>
   <si>
@@ -205,6 +205,9 @@
     <t>Sevenoaks District Council</t>
   </si>
   <si>
+    <t>Adur District Council</t>
+  </si>
+  <si>
     <t>Basingstoke and Deane Borough Council</t>
   </si>
   <si>
@@ -217,18 +220,15 @@
     <t>St Albans City and District Council</t>
   </si>
   <si>
+    <t>Worthing Borough Council</t>
+  </si>
+  <si>
     <t>Warwick District Council</t>
   </si>
   <si>
     <t>Colchester Borough Council</t>
   </si>
   <si>
-    <t>Worthing Borough Council</t>
-  </si>
-  <si>
-    <t>Adur District Council</t>
-  </si>
-  <si>
     <t>Ipswich Borough Council</t>
   </si>
   <si>
@@ -442,12 +442,12 @@
     <t>Chelmsford City Council</t>
   </si>
   <si>
+    <t>Test Valley Borough Council</t>
+  </si>
+  <si>
     <t>Hambleton District Council</t>
   </si>
   <si>
-    <t>Test Valley Borough Council</t>
-  </si>
-  <si>
     <t>Rother District Council</t>
   </si>
   <si>
@@ -511,12 +511,12 @@
     <t>Rochford District Council</t>
   </si>
   <si>
+    <t>Vale of White Horse District Council</t>
+  </si>
+  <si>
     <t>Tamworth Borough Council</t>
   </si>
   <si>
-    <t>Vale of White Horse District Council</t>
-  </si>
-  <si>
     <t>Dartford Borough Council</t>
   </si>
   <si>
@@ -709,12 +709,12 @@
     <t>THA</t>
   </si>
   <si>
+    <t>BAB</t>
+  </si>
+  <si>
     <t>MSU</t>
   </si>
   <si>
-    <t>BAB</t>
-  </si>
-  <si>
     <t>MDE</t>
   </si>
   <si>
@@ -748,6 +748,9 @@
     <t>SEV</t>
   </si>
   <si>
+    <t>ADU</t>
+  </si>
+  <si>
     <t>BAN</t>
   </si>
   <si>
@@ -760,18 +763,15 @@
     <t>SAL</t>
   </si>
   <si>
+    <t>WOT</t>
+  </si>
+  <si>
     <t>WAW</t>
   </si>
   <si>
     <t>COL</t>
   </si>
   <si>
-    <t>WOT</t>
-  </si>
-  <si>
-    <t>ADU</t>
-  </si>
-  <si>
     <t>IPS</t>
   </si>
   <si>
@@ -985,12 +985,12 @@
     <t>CHL</t>
   </si>
   <si>
+    <t>TES</t>
+  </si>
+  <si>
     <t>HAE</t>
   </si>
   <si>
-    <t>TES</t>
-  </si>
-  <si>
     <t>ROH</t>
   </si>
   <si>
@@ -1054,10 +1054,10 @@
     <t>ROC</t>
   </si>
   <si>
+    <t>VAL</t>
+  </si>
+  <si>
     <t>TAW</t>
-  </si>
-  <si>
-    <t>VAL</t>
   </si>
   <si>
     <t>DAR</t>
@@ -3409,16 +3409,16 @@
         <v>0.5779761904761905</v>
       </c>
       <c r="O31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P31" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="Q31" t="s">
         <v>394</v>
       </c>
       <c r="R31" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="S31" t="s">
         <v>402</v>
@@ -3468,16 +3468,16 @@
         <v>0.5779761904761905</v>
       </c>
       <c r="O32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P32" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="Q32" t="s">
         <v>394</v>
       </c>
       <c r="R32" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="S32" t="s">
         <v>402</v>
@@ -4149,43 +4149,43 @@
         <v>0.6190476190476191</v>
       </c>
       <c r="F44">
-        <v>0.4444444444444444</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G44">
-        <v>0.8571428571428571</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="H44">
         <v>0.5555555555555556</v>
       </c>
       <c r="I44">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="J44">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="K44">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="L44">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="M44">
         <v>0.5</v>
       </c>
       <c r="N44">
-        <v>0.5414285714285715</v>
+        <v>0.5415476190476191</v>
       </c>
       <c r="O44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P44" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="Q44" t="s">
         <v>392</v>
       </c>
       <c r="R44" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="S44" t="s">
         <v>403</v>
@@ -4205,22 +4205,22 @@
         <v>245</v>
       </c>
       <c r="E45">
-        <v>0.6666666666666666</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F45">
-        <v>0.2777777777777778</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="G45">
-        <v>0.7142857142857143</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="H45">
-        <v>0.6666666666666666</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J45">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -4229,19 +4229,19 @@
         <v>0.4</v>
       </c>
       <c r="M45">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N45">
-        <v>0.5388095238095237</v>
+        <v>0.5414285714285715</v>
       </c>
       <c r="O45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P45" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="Q45" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="R45" t="s">
         <v>397</v>
@@ -4264,34 +4264,34 @@
         <v>246</v>
       </c>
       <c r="E46">
-        <v>0.6190476190476191</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F46">
-        <v>0.5</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="G46">
-        <v>0.8571428571428571</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="H46">
-        <v>0.5555555555555556</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I46">
         <v>1</v>
       </c>
       <c r="J46">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="M46">
         <v>0.25</v>
       </c>
       <c r="N46">
-        <v>0.5372619047619047</v>
+        <v>0.5388095238095237</v>
       </c>
       <c r="O46">
         <v>2</v>
@@ -4306,7 +4306,7 @@
         <v>397</v>
       </c>
       <c r="S46" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="47" spans="1:19">
@@ -4323,19 +4323,19 @@
         <v>247</v>
       </c>
       <c r="E47">
-        <v>0.5714285714285714</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F47">
-        <v>0.6666666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="G47">
-        <v>0.4285714285714285</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="H47">
-        <v>0.7777777777777778</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="I47">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J47">
         <v>0.5</v>
@@ -4344,28 +4344,28 @@
         <v>0</v>
       </c>
       <c r="L47">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="M47">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="N47">
-        <v>0.5291666666666667</v>
+        <v>0.5372619047619047</v>
       </c>
       <c r="O47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P47" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="Q47" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="R47" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="S47" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:19">
@@ -4382,19 +4382,19 @@
         <v>248</v>
       </c>
       <c r="E48">
-        <v>0.9047619047619048</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="F48">
-        <v>0.5555555555555556</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G48">
         <v>0.4285714285714285</v>
       </c>
       <c r="H48">
-        <v>0.6666666666666666</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="I48">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="J48">
         <v>0.5</v>
@@ -4403,28 +4403,28 @@
         <v>0</v>
       </c>
       <c r="L48">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="M48">
         <v>0.75</v>
       </c>
       <c r="N48">
-        <v>0.5258333333333334</v>
+        <v>0.5291666666666667</v>
       </c>
       <c r="O48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P48" t="s">
         <v>383</v>
       </c>
       <c r="Q48" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="R48" t="s">
         <v>400</v>
       </c>
       <c r="S48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="49" spans="1:19">
@@ -4441,49 +4441,49 @@
         <v>249</v>
       </c>
       <c r="E49">
-        <v>0.4761904761904762</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F49">
-        <v>0.2777777777777778</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G49">
-        <v>0.8571428571428571</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="H49">
-        <v>0.6666666666666666</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="I49">
         <v>0.6</v>
       </c>
       <c r="J49">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="K49">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="L49">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="M49">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="N49">
-        <v>0.5166666666666666</v>
+        <v>0.529047619047619</v>
       </c>
       <c r="O49">
         <v>3</v>
       </c>
       <c r="P49" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="Q49" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="R49" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="S49" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="50" spans="1:19">
@@ -4500,49 +4500,49 @@
         <v>250</v>
       </c>
       <c r="E50">
-        <v>0.6190476190476191</v>
+        <v>0.9047619047619048</v>
       </c>
       <c r="F50">
         <v>0.5555555555555556</v>
       </c>
       <c r="G50">
-        <v>0.2857142857142857</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="H50">
-        <v>0.5555555555555556</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I50">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="J50">
+        <v>0.5</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
         <v>0.75</v>
       </c>
-      <c r="K50">
-        <v>0.4</v>
-      </c>
-      <c r="L50">
-        <v>0.6</v>
-      </c>
-      <c r="M50">
-        <v>0.25</v>
-      </c>
       <c r="N50">
-        <v>0.5123809523809524</v>
+        <v>0.5258333333333334</v>
       </c>
       <c r="O50">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P50" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="Q50" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="R50" t="s">
         <v>400</v>
       </c>
       <c r="S50" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="51" spans="1:19">
@@ -4559,49 +4559,49 @@
         <v>251</v>
       </c>
       <c r="E51">
-        <v>0.6190476190476191</v>
+        <v>0.4761904761904762</v>
       </c>
       <c r="F51">
-        <v>0.5555555555555556</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="G51">
-        <v>0.2857142857142857</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="H51">
-        <v>0.5555555555555556</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I51">
         <v>0.6</v>
       </c>
       <c r="J51">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
         <v>0.4</v>
       </c>
-      <c r="L51">
-        <v>0.6</v>
-      </c>
       <c r="M51">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N51">
-        <v>0.5123809523809524</v>
+        <v>0.5166666666666666</v>
       </c>
       <c r="O51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P51" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="Q51" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="R51" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="S51" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="52" spans="1:19">
@@ -8807,31 +8807,31 @@
         <v>323</v>
       </c>
       <c r="E123">
-        <v>0.1904761904761905</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F123">
-        <v>0.1666666666666667</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="G123">
-        <v>0.4285714285714285</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="H123">
-        <v>0.3333333333333333</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="I123">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J123">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K123">
         <v>0</v>
       </c>
       <c r="L123">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="M123">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="N123">
         <v>0.2203571428571429</v>
@@ -8840,13 +8840,13 @@
         <v>4</v>
       </c>
       <c r="P123" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="Q123" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="R123" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S123" t="s">
         <v>403</v>
@@ -8866,31 +8866,31 @@
         <v>324</v>
       </c>
       <c r="E124">
+        <v>0.1904761904761905</v>
+      </c>
+      <c r="F124">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="G124">
+        <v>0.4285714285714285</v>
+      </c>
+      <c r="H124">
         <v>0.3333333333333333</v>
       </c>
-      <c r="F124">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="G124">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H124">
-        <v>0.4444444444444444</v>
-      </c>
       <c r="I124">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>0.2</v>
+      </c>
+      <c r="M124">
         <v>0.25</v>
-      </c>
-      <c r="K124">
-        <v>0</v>
-      </c>
-      <c r="L124">
-        <v>0</v>
-      </c>
-      <c r="M124">
-        <v>0</v>
       </c>
       <c r="N124">
         <v>0.2203571428571429</v>
@@ -8899,13 +8899,13 @@
         <v>4</v>
       </c>
       <c r="P124" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="Q124" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="R124" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="S124" t="s">
         <v>403</v>
@@ -10194,19 +10194,19 @@
         <v>0</v>
       </c>
       <c r="O146">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P146" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="Q146" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="R146" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="S146" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="147" spans="1:19">
@@ -10253,19 +10253,19 @@
         <v>0</v>
       </c>
       <c r="O147">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P147" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="Q147" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="R147" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="S147" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="148" spans="1:19">

</xml_diff>